<commit_message>
VISTA-5923: Updated building utilities for preload process
</commit_message>
<xml_diff>
--- a/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/util/building-utilities.xlsx
+++ b/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/util/building-utilities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="143" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="203" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,49 +35,49 @@
     <t>Last technology in temperature control on all public building places</t>
   </si>
   <si>
-    <t>internet</t>
-  </si>
-  <si>
-    <t>Public Internet</t>
-  </si>
-  <si>
-    <t>Room with high speed Internet connection on the main hall is available</t>
-  </si>
-  <si>
-    <t>garbage</t>
-  </si>
-  <si>
-    <t>Garbage Disposal</t>
-  </si>
-  <si>
-    <t>Built-in garbage collection on all floors</t>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Last technology pipes, granted heat water even during the winter </t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>Granted electric power supply 365 days a year </t>
   </si>
   <si>
     <t>electricity</t>
   </si>
   <si>
-    <t>Granted electricity</t>
+    <t>Electricity</t>
   </si>
   <si>
     <t>Power generator grants electricity for 48 hours after some power cut</t>
   </si>
   <si>
-    <t>television</t>
-  </si>
-  <si>
-    <t>TV on hall</t>
-  </si>
-  <si>
-    <t>Guests waiting room includes 48 inches TV</t>
-  </si>
-  <si>
-    <t>telephone</t>
-  </si>
-  <si>
-    <t>Public telephone</t>
-  </si>
-  <si>
-    <t>Public telephone available</t>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Gas burners included in the kitchen and balcony </t>
+  </si>
+  <si>
+    <t>airConditioning</t>
+  </si>
+  <si>
+    <t>Air Conditioning</t>
+  </si>
+  <si>
+    <t>Great savings for your summer bills!! Intelligent system of air conditioning in all rooms </t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,6 @@
       <family val="0"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -198,13 +197,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2295918367347"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -230,7 +230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -263,7 +263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -274,7 +274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>